<commit_message>
05-02-2025 Q1 scripts, MDI, overfitting check
</commit_message>
<xml_diff>
--- a/analysis/results/Q1/alpha_diversity/alpha_diversity_results_colon.xlsx
+++ b/analysis/results/Q1/alpha_diversity/alpha_diversity_results_colon.xlsx
@@ -41,19 +41,19 @@
     <t xml:space="preserve">sig</t>
   </si>
   <si>
-    <t xml:space="preserve">pre_ltx vs Grouphealthy</t>
+    <t xml:space="preserve">healthy vs Grouppre_ltx</t>
   </si>
   <si>
     <t xml:space="preserve">***</t>
   </si>
   <si>
-    <t xml:space="preserve">pre_ltx vs healthy - CZ vs NO</t>
+    <t xml:space="preserve">healthy vs pre_ltx - CZ vs NO</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">pre_ltx vs Grouphealthy:CountryNO</t>
+    <t xml:space="preserve">healthy vs Grouppre_ltx:CountryNO</t>
   </si>
   <si>
     <t xml:space="preserve">pre_ltx vs Grouppost_ltx</t>
@@ -68,16 +68,16 @@
     <t xml:space="preserve">pre_ltx vs Grouppost_ltx:CountryNO</t>
   </si>
   <si>
-    <t xml:space="preserve">post_ltx vs Grouphealthy</t>
+    <t xml:space="preserve">healthy vs Grouppost_ltx</t>
   </si>
   <si>
     <t xml:space="preserve">**</t>
   </si>
   <si>
-    <t xml:space="preserve">post_ltx vs healthy - CZ vs NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post_ltx vs Grouphealthy:CountryNO</t>
+    <t xml:space="preserve">healthy vs post_ltx - CZ vs NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">healthy vs Grouppost_ltx:CountryNO</t>
   </si>
 </sst>
 </file>
@@ -440,22 +440,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>56.2297874111756</v>
+        <v>-56.2297874111623</v>
       </c>
       <c r="C2" t="n">
-        <v>11.7376584504173</v>
+        <v>11.7376584507647</v>
       </c>
       <c r="D2" t="n">
-        <v>195.570182204725</v>
+        <v>195.570180915709</v>
       </c>
       <c r="E2" t="n">
-        <v>4.79054554609028</v>
+        <v>-4.79054554594736</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0000032810003037713</v>
+        <v>0.00000328100031952592</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000295290027339417</v>
+        <v>0.0000295290028757333</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -466,22 +466,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>6.70373494971469</v>
+        <v>14.1930992929996</v>
       </c>
       <c r="C3" t="n">
-        <v>11.0979246747831</v>
+        <v>10.3411147337777</v>
       </c>
       <c r="D3" t="n">
-        <v>194.202342036778</v>
+        <v>194.537858584009</v>
       </c>
       <c r="E3" t="n">
-        <v>0.604053023079805</v>
+        <v>1.37249219821921</v>
       </c>
       <c r="F3" t="n">
-        <v>0.546513372422205</v>
+        <v>0.171490557299805</v>
       </c>
       <c r="G3" t="n">
-        <v>0.622058607047551</v>
+        <v>0.255969836828398</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -492,22 +492,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>7.48936434330525</v>
+        <v>-7.48936434332061</v>
       </c>
       <c r="C4" t="n">
-        <v>15.1691326719083</v>
+        <v>15.1691326723597</v>
       </c>
       <c r="D4" t="n">
-        <v>194.358195676071</v>
+        <v>194.358194950027</v>
       </c>
       <c r="E4" t="n">
-        <v>0.493723965983553</v>
+        <v>-0.493723965969872</v>
       </c>
       <c r="F4" t="n">
-        <v>0.622058607047551</v>
+        <v>0.622058607059278</v>
       </c>
       <c r="G4" t="n">
-        <v>0.622058607047551</v>
+        <v>0.622058607059278</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -559,7 +559,7 @@
         <v>0.580161717393637</v>
       </c>
       <c r="G6" t="n">
-        <v>0.622058607047551</v>
+        <v>0.622058607059278</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -585,7 +585,7 @@
         <v>0.112754329652137</v>
       </c>
       <c r="G7" t="n">
-        <v>0.169131494478205</v>
+        <v>0.202957793373846</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -596,22 +596,22 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>27.2991489166295</v>
+        <v>-27.299148916624</v>
       </c>
       <c r="C8" t="n">
-        <v>8.69854137378727</v>
+        <v>8.69854137378728</v>
       </c>
       <c r="D8" t="n">
-        <v>250.458337518235</v>
+        <v>250.458335818147</v>
       </c>
       <c r="E8" t="n">
-        <v>3.13835938044676</v>
+        <v>-3.13835938044611</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00190243832157631</v>
+        <v>0.0019024383230054</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00856097244709339</v>
+        <v>0.00856097245352429</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -622,22 +622,22 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>-17.3210386346946</v>
+        <v>14.3603645603166</v>
       </c>
       <c r="C9" t="n">
-        <v>8.7806945453549</v>
+        <v>11.1533109482603</v>
       </c>
       <c r="D9" t="n">
-        <v>240.908571083271</v>
+        <v>251.728796047421</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.97262739812053</v>
+        <v>1.28754274196547</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0496815576868389</v>
+        <v>0.199087650866532</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0894268038363101</v>
+        <v>0.255969836828398</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -648,22 +648,22 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>31.681403195004</v>
+        <v>-31.6814031950151</v>
       </c>
       <c r="C10" t="n">
-        <v>14.1949618459299</v>
+        <v>14.19496184593</v>
       </c>
       <c r="D10" t="n">
-        <v>247.530840688515</v>
+        <v>247.530840100213</v>
       </c>
       <c r="E10" t="n">
-        <v>2.23187660092851</v>
+        <v>-2.23187660092929</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0265186605221946</v>
+        <v>0.0265186605242804</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0596669861749378</v>
+        <v>0.0596669861796309</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -714,22 +714,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.58463871613819</v>
+        <v>-0.584638716137957</v>
       </c>
       <c r="C2" t="n">
-        <v>0.143155036380832</v>
+        <v>0.143155036381466</v>
       </c>
       <c r="D2" t="n">
-        <v>197.587542707025</v>
+        <v>197.587543805541</v>
       </c>
       <c r="E2" t="n">
-        <v>4.08395492690101</v>
+        <v>-4.08395492688128</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0000642923959062244</v>
+        <v>0.0000642923957847682</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00057863156315602</v>
+        <v>0.000578631562062914</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -740,22 +740,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0954458173398966</v>
+        <v>0.0146781534706523</v>
       </c>
       <c r="C3" t="n">
-        <v>0.135270221509658</v>
+        <v>0.126064800286197</v>
       </c>
       <c r="D3" t="n">
-        <v>195.749967545478</v>
+        <v>196.213354178243</v>
       </c>
       <c r="E3" t="n">
-        <v>0.705593709204371</v>
+        <v>0.116433401213736</v>
       </c>
       <c r="F3" t="n">
-        <v>0.481279662242131</v>
+        <v>0.907428148748997</v>
       </c>
       <c r="G3" t="n">
-        <v>0.618788137168454</v>
+        <v>0.909474207145245</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -766,22 +766,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0807676638697057</v>
+        <v>0.0807676638695282</v>
       </c>
       <c r="C4" t="n">
-        <v>0.184906372789929</v>
+        <v>0.184906372790758</v>
       </c>
       <c r="D4" t="n">
-        <v>195.965217414699</v>
+        <v>195.965218122722</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.436803029831024</v>
+        <v>0.436803029828105</v>
       </c>
       <c r="F4" t="n">
-        <v>0.662735115053286</v>
+        <v>0.662735115053663</v>
       </c>
       <c r="G4" t="n">
-        <v>0.662735115053286</v>
+        <v>0.852088005068996</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -807,10 +807,10 @@
         <v>0.0218441469197754</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0451834116960333</v>
+        <v>0.0564792646200416</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -833,7 +833,7 @@
         <v>0.559038373247334</v>
       </c>
       <c r="G6" t="n">
-        <v>0.628918169903251</v>
+        <v>0.838557559871001</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -859,10 +859,10 @@
         <v>0.0251018953866852</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0451834116960333</v>
+        <v>0.0564792646200416</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -870,25 +870,25 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.219739423027333</v>
+        <v>-0.219739423568967</v>
       </c>
       <c r="C8" t="n">
-        <v>0.102071457793904</v>
+        <v>0.102071461452386</v>
       </c>
       <c r="D8" t="n">
-        <v>247.58565962123</v>
+        <v>247.585634183915</v>
       </c>
       <c r="E8" t="n">
-        <v>2.15279988918172</v>
+        <v>-2.1527998173267</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0323009058211522</v>
+        <v>0.0323009116336897</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0484513587317282</v>
+        <v>0.0581416409406414</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -896,25 +896,25 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.360831428253397</v>
+        <v>0.0148944623604509</v>
       </c>
       <c r="C9" t="n">
-        <v>0.103119472283225</v>
+        <v>0.130862581417962</v>
       </c>
       <c r="D9" t="n">
-        <v>238.824197064494</v>
+        <v>248.75891335263</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.49915898776468</v>
+        <v>0.113817580236168</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00055662543545193</v>
+        <v>0.909474207145245</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00250481445953368</v>
+        <v>0.909474207145245</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -922,25 +922,25 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>0.375725891037435</v>
+        <v>-0.375725890122552</v>
       </c>
       <c r="C10" t="n">
-        <v>0.166609242112832</v>
+        <v>0.166609248148072</v>
       </c>
       <c r="D10" t="n">
-        <v>244.903563802815</v>
+        <v>244.90353833122</v>
       </c>
       <c r="E10" t="n">
-        <v>2.25513234603746</v>
+        <v>-2.25513225885654</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0250086127454535</v>
+        <v>0.0250086183896467</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0451834116960333</v>
+        <v>0.0564792646200416</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -988,22 +988,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0586931376058512</v>
+        <v>-0.058693137605951</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0191445452133138</v>
+        <v>0.0191445452131798</v>
       </c>
       <c r="D2" t="n">
-        <v>199.853177893729</v>
+        <v>199.8531786722</v>
       </c>
       <c r="E2" t="n">
-        <v>3.06578907735212</v>
+        <v>-3.06578907737878</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00247109030136223</v>
+        <v>0.00247109029994167</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0222398127122601</v>
+        <v>0.0222398126994751</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -1014,22 +1014,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0128473440791356</v>
+        <v>-0.00725094013991043</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0180785210558815</v>
+        <v>0.0168510078148344</v>
       </c>
       <c r="D3" t="n">
-        <v>197.522448854834</v>
+        <v>198.127375767928</v>
       </c>
       <c r="E3" t="n">
-        <v>0.710641320682366</v>
+        <v>-0.430297120480072</v>
       </c>
       <c r="F3" t="n">
-        <v>0.478144772278227</v>
+        <v>0.667447205149642</v>
       </c>
       <c r="G3" t="n">
-        <v>0.537912868813005</v>
+        <v>0.737867463605542</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -1040,22 +1040,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.020098284218957</v>
+        <v>0.0200982842190763</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0247141535956133</v>
+        <v>0.0247141535954386</v>
       </c>
       <c r="D4" t="n">
-        <v>197.80344353466</v>
+        <v>197.803443913675</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.81322972041917</v>
+        <v>0.813229720429746</v>
       </c>
       <c r="F4" t="n">
-        <v>0.417064141588458</v>
+        <v>0.417064141580538</v>
       </c>
       <c r="G4" t="n">
-        <v>0.536225324899446</v>
+        <v>0.625596212370807</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -1081,7 +1081,7 @@
         <v>0.226307934159494</v>
       </c>
       <c r="G5" t="n">
-        <v>0.378927402160893</v>
+        <v>0.45471288265286</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -1107,7 +1107,7 @@
         <v>0.634709253913446</v>
       </c>
       <c r="G6" t="n">
-        <v>0.634709253913446</v>
+        <v>0.737867463605542</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -1133,7 +1133,7 @@
         <v>0.120851069495904</v>
       </c>
       <c r="G7" t="n">
-        <v>0.271914906365785</v>
+        <v>0.362553208487713</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -1144,22 +1144,22 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0270796696675777</v>
+        <v>-0.0270796696678986</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0169835936215225</v>
+        <v>0.0169835936225165</v>
       </c>
       <c r="D8" t="n">
-        <v>246.082174127465</v>
+        <v>246.082173765515</v>
       </c>
       <c r="E8" t="n">
-        <v>1.59446052885185</v>
+        <v>-1.59446052877743</v>
       </c>
       <c r="F8" t="n">
-        <v>0.112116439268231</v>
+        <v>0.112116439286781</v>
       </c>
       <c r="G8" t="n">
-        <v>0.271914906365785</v>
+        <v>0.362553208487713</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -1170,22 +1170,22 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0390937223183898</v>
+        <v>-0.00729458643870464</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0171750014820315</v>
+        <v>0.0217712802387507</v>
       </c>
       <c r="D9" t="n">
-        <v>238.277082212576</v>
+        <v>247.135382698276</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.27619906521055</v>
+        <v>-0.335055465673581</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0237221602947391</v>
+        <v>0.737867463605542</v>
       </c>
       <c r="G9" t="n">
-        <v>0.106749721326326</v>
+        <v>0.737867463605542</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -1196,22 +1196,22 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>0.031799135879857</v>
+        <v>-0.0317991358794888</v>
       </c>
       <c r="C10" t="n">
-        <v>0.027730296051192</v>
+        <v>0.02773029605283</v>
       </c>
       <c r="D10" t="n">
-        <v>243.697487807188</v>
+        <v>243.697487853012</v>
       </c>
       <c r="E10" t="n">
-        <v>1.14672904397247</v>
+        <v>-1.14672904389146</v>
       </c>
       <c r="F10" t="n">
-        <v>0.252618268107262</v>
+        <v>0.252618268140478</v>
       </c>
       <c r="G10" t="n">
-        <v>0.378927402160893</v>
+        <v>0.45471288265286</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -1262,22 +1262,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.056958637808368</v>
+        <v>-0.0569586378083008</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0201379137971606</v>
+        <v>0.0201379137971631</v>
       </c>
       <c r="D2" t="n">
-        <v>201.12982296481</v>
+        <v>201.129821433303</v>
       </c>
       <c r="E2" t="n">
-        <v>2.82842792863673</v>
+        <v>-2.82842792863304</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0051511760028923</v>
+        <v>0.00515117600663822</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0231802920130153</v>
+        <v>0.046360584059744</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -1288,22 +1288,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0067822681680891</v>
+        <v>-0.00790346060303697</v>
       </c>
       <c r="C3" t="n">
-        <v>0.019002848847414</v>
+        <v>0.0177159654026436</v>
       </c>
       <c r="D3" t="n">
-        <v>198.242715507883</v>
+        <v>199.016528896297</v>
       </c>
       <c r="E3" t="n">
-        <v>0.356907967986708</v>
+        <v>-0.44612079688627</v>
       </c>
       <c r="F3" t="n">
-        <v>0.721540320773647</v>
+        <v>0.655994977824663</v>
       </c>
       <c r="G3" t="n">
-        <v>0.784623196091076</v>
+        <v>0.78097352770903</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -1314,22 +1314,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0146857287711355</v>
+        <v>0.014685728771077</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0259800634037961</v>
+        <v>0.0259800634037992</v>
       </c>
       <c r="D4" t="n">
-        <v>198.602151889824</v>
+        <v>198.602151099978</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.565269165932433</v>
+        <v>0.565269165930113</v>
       </c>
       <c r="F4" t="n">
-        <v>0.572528702840476</v>
+        <v>0.572528702844586</v>
       </c>
       <c r="G4" t="n">
-        <v>0.736108332223469</v>
+        <v>0.78097352770903</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -1355,7 +1355,7 @@
         <v>0.104142067834683</v>
       </c>
       <c r="G5" t="n">
-        <v>0.187455722102429</v>
+        <v>0.234319652628036</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -1407,7 +1407,7 @@
         <v>0.0449642903158472</v>
       </c>
       <c r="G7" t="n">
-        <v>0.134892870947542</v>
+        <v>0.202339306421313</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -1418,22 +1418,22 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0178562322308381</v>
+        <v>-0.0178562322308237</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0158041262924136</v>
+        <v>0.0158041262922856</v>
       </c>
       <c r="D8" t="n">
-        <v>247.07616247913</v>
+        <v>247.076162786932</v>
       </c>
       <c r="E8" t="n">
-        <v>1.12984621234073</v>
+        <v>-1.12984621234897</v>
       </c>
       <c r="F8" t="n">
-        <v>0.259636697005352</v>
+        <v>0.259636697000521</v>
       </c>
       <c r="G8" t="n">
-        <v>0.389455045508029</v>
+        <v>0.467346054600939</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -1444,25 +1444,25 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0550996033407275</v>
+        <v>-0.0079773077315203</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0159390532667313</v>
+        <v>0.0202664850400594</v>
       </c>
       <c r="D9" t="n">
-        <v>236.677505226214</v>
+        <v>248.451075779612</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.45689310517168</v>
+        <v>-0.393620685370556</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000647673686435841</v>
+        <v>0.694198691296915</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00582906317792257</v>
+        <v>0.78097352770903</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -1470,22 +1470,22 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>0.047122295609225</v>
+        <v>-0.0471222956091828</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0257834023147697</v>
+        <v>0.0257834023145581</v>
       </c>
       <c r="D10" t="n">
-        <v>243.881388474435</v>
+        <v>243.881388465963</v>
       </c>
       <c r="E10" t="n">
-        <v>1.82762131366316</v>
+        <v>-1.82762131367651</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0688282457304898</v>
+        <v>0.0688282457285189</v>
       </c>
       <c r="G10" t="n">
-        <v>0.154863552893602</v>
+        <v>0.206484737185557</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>

</xml_diff>